<commit_message>
Added a missing interval in schedule template test file
</commit_message>
<xml_diff>
--- a/src/main/resources/com/endava/tmd/soj/scheduleTemplate.xlsx
+++ b/src/main/resources/com/endava/tmd/soj/scheduleTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrutodea/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrutodea/dev/schedule-matcher/src/main/resources/com/endava/tmd/soj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CF9C2F4-2B55-4B4D-81C0-B7322C4BDA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C746DD1-7E74-1144-A003-9D646BFA8CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{908E9387-ABF5-9B43-AAD6-F9C58C7F893A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Monday</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>18:00 - 19:00</t>
+  </si>
+  <si>
+    <t>16:00 - 17:00</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DE7AB4-C00E-AF44-A2EC-23C788DC93FF}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,15 +516,21 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>